<commit_message>
Finalizing upload of alpha data preanalysis
</commit_message>
<xml_diff>
--- a/Simulations/SRIM_AlphasVsFilters/DataAnalysis/ThinFilter_Analysis.xlsx
+++ b/Simulations/SRIM_AlphasVsFilters/DataAnalysis/ThinFilter_Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giova\Documents\GitHub\xmm-newton\Simulations\SRIM_AlphasVsFilters\DataAnalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23CF57A5-576D-4E1F-A395-C9AF877BA480}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14F5E770-0C40-414D-BDFB-3193D3932B2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A9EDBC4B-5209-4052-BD5C-CBCCBA64D68C}"/>
   </bookViews>
@@ -67,18 +67,19 @@
     <t>Error on mean energy loss [keV]</t>
   </si>
   <si>
-    <t>Number of ions passed [%]</t>
+    <t>Number of ions transmitted [%]</t>
   </si>
   <si>
-    <t>ALPHA PARTICLES VS THIN FILTER</t>
+    <t>ALPHA PARTICLES VS THIN FILTERS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -154,7 +155,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -172,6 +173,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="166" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -506,46 +508,46 @@
                 <c:pt idx="1">
                   <c:v>0.40566559777777778</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="2" formatCode="0.0">
                   <c:v>4.1516317468317965</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="3" formatCode="0.0">
                   <c:v>10.460844563862253</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="4" formatCode="0.0">
                   <c:v>17.46051739</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="5" formatCode="0.0">
                   <c:v>24.931449690000001</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="6" formatCode="0.0">
                   <c:v>32.640090069999999</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="7" formatCode="0.0">
                   <c:v>40.630279689482684</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="8" formatCode="0.0">
                   <c:v>48.85064242</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="9" formatCode="0.0">
                   <c:v>57.191133479999998</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="10" formatCode="0.0">
                   <c:v>65.636556049999996</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="11" formatCode="0.0">
                   <c:v>82.738911859999988</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="12" formatCode="0.0">
                   <c:v>100.0572885</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="13" formatCode="0.0">
                   <c:v>117.53107300000001</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="14" formatCode="0.0">
                   <c:v>135.4214546</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="15" formatCode="0.0">
                   <c:v>153.37181989999999</c:v>
                 </c:pt>
               </c:numCache>
@@ -1159,9 +1161,9 @@
             <c:numRef>
               <c:f>Foglio1!$G$6:$G$21</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="16"/>
-                <c:pt idx="0">
+                <c:pt idx="0" formatCode="0.00">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
@@ -1878,9 +1880,9 @@
             <c:numRef>
               <c:f>Foglio1!$C$7:$C$21</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="15"/>
-                <c:pt idx="0">
+                <c:pt idx="0" formatCode="0.00">
                   <c:v>0.40566559777777778</c:v>
                 </c:pt>
                 <c:pt idx="1">
@@ -1932,7 +1934,7 @@
             <c:numRef>
               <c:f>Foglio1!$G$7:$G$21</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>9.5943344022222217</c:v>
@@ -2194,7 +2196,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -4368,15 +4370,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="18" customWidth="1"/>
     <col min="3" max="3" width="18.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="32.21875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.77734375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="25.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="35" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -4461,7 +4463,7 @@
       <c r="A6" s="3">
         <v>1</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="6">
         <v>0</v>
       </c>
       <c r="C6" s="4">
@@ -4494,7 +4496,7 @@
       <c r="A7" s="3">
         <v>10</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="6">
         <v>405.66559777777775</v>
       </c>
       <c r="C7" s="4">
@@ -4512,11 +4514,11 @@
         <f>E7/C7</f>
         <v>0.55543884466048177</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="11">
         <f t="shared" ref="G7:G21" si="2">A7-C7</f>
         <v>9.5943344022222217</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H7" s="11">
         <f t="shared" ref="H7:H21" si="3">F7*G7</f>
         <v>5.3290660156566245</v>
       </c>
@@ -4529,17 +4531,17 @@
       <c r="A8" s="3">
         <v>20</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="6">
         <v>4151.6317468317966</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="11">
         <f t="shared" si="0"/>
         <v>4.1516317468317965</v>
       </c>
       <c r="D8" s="6">
         <v>1354.2955825473875</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="11">
         <f t="shared" si="1"/>
         <v>1.3542955825473875</v>
       </c>
@@ -4547,11 +4549,11 @@
         <f t="shared" ref="F8:F21" si="4">E8/C8</f>
         <v>0.32620802256387044</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="11">
         <f t="shared" si="2"/>
         <v>15.848368253168204</v>
       </c>
-      <c r="H8" s="4">
+      <c r="H8" s="11">
         <f t="shared" si="3"/>
         <v>5.1698648687300208</v>
       </c>
@@ -4563,17 +4565,17 @@
       <c r="A9" s="3">
         <v>30</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="6">
         <v>10460.844563862252</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="11">
         <f t="shared" si="0"/>
         <v>10.460844563862253</v>
       </c>
       <c r="D9" s="6">
         <v>1881.1518467942069</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="11">
         <f t="shared" si="1"/>
         <v>1.881151846794207</v>
       </c>
@@ -4581,11 +4583,11 @@
         <f t="shared" si="4"/>
         <v>0.1798279130628499</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="11">
         <f t="shared" si="2"/>
         <v>19.539155436137747</v>
       </c>
-      <c r="H9" s="4">
+      <c r="H9" s="11">
         <f t="shared" si="3"/>
         <v>3.5136855450912896</v>
       </c>
@@ -4597,17 +4599,17 @@
       <c r="A10" s="3">
         <v>40</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="6">
         <v>17460.517390000001</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="11">
         <f t="shared" si="0"/>
         <v>17.46051739</v>
       </c>
       <c r="D10" s="6">
         <v>2123.048769</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="11">
         <f t="shared" si="1"/>
         <v>2.1230487689999999</v>
       </c>
@@ -4615,11 +4617,11 @@
         <f t="shared" si="4"/>
         <v>0.12159140084909019</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10" s="11">
         <f t="shared" si="2"/>
         <v>22.53948261</v>
       </c>
-      <c r="H10" s="4">
+      <c r="H10" s="11">
         <f t="shared" si="3"/>
         <v>2.7406072649636077</v>
       </c>
@@ -4631,17 +4633,17 @@
       <c r="A11" s="3">
         <v>50</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11" s="6">
         <v>24931.449690000001</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="11">
         <f t="shared" si="0"/>
         <v>24.931449690000001</v>
       </c>
       <c r="D11" s="6">
         <v>2031.020994</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="11">
         <f t="shared" si="1"/>
         <v>2.0310209939999999</v>
       </c>
@@ -4649,11 +4651,11 @@
         <f t="shared" si="4"/>
         <v>8.1464215649467112E-2</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G11" s="11">
         <f t="shared" si="2"/>
         <v>25.068550309999999</v>
       </c>
-      <c r="H11" s="4">
+      <c r="H11" s="11">
         <f t="shared" si="3"/>
         <v>2.0421897884733555</v>
       </c>
@@ -4665,17 +4667,17 @@
       <c r="A12" s="3">
         <v>60</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="6">
         <v>32640.090069999998</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="11">
         <f>B12/1000</f>
         <v>32.640090069999999</v>
       </c>
       <c r="D12" s="6">
         <v>2206.641717</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="11">
         <f t="shared" si="1"/>
         <v>2.2066417170000001</v>
       </c>
@@ -4683,11 +4685,11 @@
         <f t="shared" si="4"/>
         <v>6.7605258204485097E-2</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G12" s="11">
         <f t="shared" si="2"/>
         <v>27.359909930000001</v>
       </c>
-      <c r="H12" s="4">
+      <c r="H12" s="11">
         <f t="shared" si="3"/>
         <v>1.8496737752691059</v>
       </c>
@@ -4699,17 +4701,17 @@
       <c r="A13" s="3">
         <v>70</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13" s="6">
         <v>40630.279689482682</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13" s="11">
         <f t="shared" si="0"/>
         <v>40.630279689482684</v>
       </c>
       <c r="D13" s="6">
         <v>2347.4836158257376</v>
       </c>
-      <c r="E13" s="4">
+      <c r="E13" s="11">
         <f t="shared" si="1"/>
         <v>2.3474836158257375</v>
       </c>
@@ -4717,11 +4719,11 @@
         <f t="shared" si="4"/>
         <v>5.7776703329792567E-2</v>
       </c>
-      <c r="G13" s="4">
+      <c r="G13" s="11">
         <f t="shared" si="2"/>
         <v>29.369720310517316</v>
       </c>
-      <c r="H13" s="4">
+      <c r="H13" s="11">
         <f t="shared" si="3"/>
         <v>1.6968856172597422</v>
       </c>
@@ -4733,17 +4735,17 @@
       <c r="A14" s="3">
         <v>80</v>
       </c>
-      <c r="B14" s="4">
+      <c r="B14" s="6">
         <v>48850.642419999996</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C14" s="11">
         <f t="shared" si="0"/>
         <v>48.85064242</v>
       </c>
       <c r="D14" s="6">
         <v>2406.3289880000002</v>
       </c>
-      <c r="E14" s="4">
+      <c r="E14" s="11">
         <f t="shared" si="1"/>
         <v>2.4063289880000003</v>
       </c>
@@ -4751,11 +4753,11 @@
         <f t="shared" si="4"/>
         <v>4.9258901598698779E-2</v>
       </c>
-      <c r="G14" s="4">
+      <c r="G14" s="11">
         <f t="shared" si="2"/>
         <v>31.14935758</v>
       </c>
-      <c r="H14" s="4">
+      <c r="H14" s="11">
         <f t="shared" si="3"/>
         <v>1.534383139895902</v>
       </c>
@@ -4767,17 +4769,17 @@
       <c r="A15" s="3">
         <v>90</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B15" s="6">
         <v>57191.133479999997</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15" s="11">
         <f t="shared" si="0"/>
         <v>57.191133479999998</v>
       </c>
       <c r="D15" s="6">
         <v>2340.6259070000001</v>
       </c>
-      <c r="E15" s="4">
+      <c r="E15" s="11">
         <f t="shared" si="1"/>
         <v>2.3406259070000002</v>
       </c>
@@ -4785,11 +4787,11 @@
         <f t="shared" si="4"/>
         <v>4.0926377299700271E-2</v>
       </c>
-      <c r="G15" s="4">
+      <c r="G15" s="11">
         <f t="shared" si="2"/>
         <v>32.808866520000002</v>
       </c>
-      <c r="H15" s="4">
+      <c r="H15" s="11">
         <f t="shared" si="3"/>
         <v>1.3427480499730244</v>
       </c>
@@ -4801,17 +4803,17 @@
       <c r="A16" s="3">
         <v>100</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B16" s="6">
         <v>65636.556049999999</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C16" s="11">
         <f t="shared" si="0"/>
         <v>65.636556049999996</v>
       </c>
       <c r="D16" s="6">
         <v>2357.0908949999998</v>
       </c>
-      <c r="E16" s="4">
+      <c r="E16" s="11">
         <f t="shared" si="1"/>
         <v>2.3570908949999998</v>
       </c>
@@ -4819,11 +4821,11 @@
         <f t="shared" si="4"/>
         <v>3.5911251851855806E-2</v>
       </c>
-      <c r="G16" s="4">
+      <c r="G16" s="11">
         <f t="shared" si="2"/>
         <v>34.363443950000004</v>
       </c>
-      <c r="H16" s="4">
+      <c r="H16" s="11">
         <f t="shared" si="3"/>
         <v>1.2340342901855808</v>
       </c>
@@ -4836,17 +4838,17 @@
         <f>A16+20</f>
         <v>120</v>
       </c>
-      <c r="B17" s="4">
+      <c r="B17" s="6">
         <v>82738.911859999993</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C17" s="11">
         <f t="shared" si="0"/>
         <v>82.738911859999988</v>
       </c>
       <c r="D17" s="6">
         <v>2327.3234560000001</v>
       </c>
-      <c r="E17" s="4">
+      <c r="E17" s="11">
         <f t="shared" si="1"/>
         <v>2.3273234560000002</v>
       </c>
@@ -4854,11 +4856,11 @@
         <f t="shared" si="4"/>
         <v>2.8128523855111776E-2</v>
       </c>
-      <c r="G17" s="4">
+      <c r="G17" s="11">
         <f t="shared" si="2"/>
         <v>37.261088140000012</v>
       </c>
-      <c r="H17" s="4">
+      <c r="H17" s="11">
         <f t="shared" si="3"/>
         <v>1.0480994066134128</v>
       </c>
@@ -4871,17 +4873,17 @@
         <f>A17+20</f>
         <v>140</v>
       </c>
-      <c r="B18" s="4">
+      <c r="B18" s="6">
         <v>100057.2885</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C18" s="11">
         <f>B18/1000</f>
         <v>100.0572885</v>
       </c>
       <c r="D18" s="6">
         <v>2392.2975179999999</v>
       </c>
-      <c r="E18" s="4">
+      <c r="E18" s="11">
         <f t="shared" si="1"/>
         <v>2.3922975179999999</v>
       </c>
@@ -4889,11 +4891,11 @@
         <f t="shared" si="4"/>
         <v>2.3909277913322625E-2</v>
       </c>
-      <c r="G18" s="4">
+      <c r="G18" s="11">
         <f t="shared" si="2"/>
         <v>39.942711500000001</v>
       </c>
-      <c r="H18" s="4">
+      <c r="H18" s="11">
         <f t="shared" si="3"/>
         <v>0.95500138986516769</v>
       </c>
@@ -4906,17 +4908,17 @@
         <f>A18+20</f>
         <v>160</v>
       </c>
-      <c r="B19" s="4">
+      <c r="B19" s="6">
         <v>117531.073</v>
       </c>
-      <c r="C19" s="4">
+      <c r="C19" s="11">
         <f t="shared" si="0"/>
         <v>117.53107300000001</v>
       </c>
       <c r="D19" s="6">
         <v>2873.4742200000001</v>
       </c>
-      <c r="E19" s="4">
+      <c r="E19" s="11">
         <f t="shared" si="1"/>
         <v>2.8734742199999999</v>
       </c>
@@ -4924,11 +4926,11 @@
         <f t="shared" si="4"/>
         <v>2.4448634277337022E-2</v>
       </c>
-      <c r="G19" s="4">
+      <c r="G19" s="11">
         <f t="shared" si="2"/>
         <v>42.468926999999994</v>
       </c>
-      <c r="H19" s="4">
+      <c r="H19" s="11">
         <f t="shared" si="3"/>
         <v>1.0383072643739235</v>
       </c>
@@ -4941,17 +4943,17 @@
         <f>A19+20</f>
         <v>180</v>
       </c>
-      <c r="B20" s="4">
+      <c r="B20" s="6">
         <v>135421.4546</v>
       </c>
-      <c r="C20" s="4">
+      <c r="C20" s="11">
         <f t="shared" si="0"/>
         <v>135.4214546</v>
       </c>
       <c r="D20" s="6">
         <v>2432.3568660000001</v>
       </c>
-      <c r="E20" s="4">
+      <c r="E20" s="11">
         <f t="shared" si="1"/>
         <v>2.4323568660000001</v>
       </c>
@@ -4959,11 +4961,11 @@
         <f t="shared" si="4"/>
         <v>1.7961384872024554E-2</v>
       </c>
-      <c r="G20" s="4">
+      <c r="G20" s="11">
         <f>A20-C20</f>
         <v>44.578545399999996</v>
       </c>
-      <c r="H20" s="4">
+      <c r="H20" s="11">
         <f t="shared" si="3"/>
         <v>0.80069241096441968</v>
       </c>
@@ -4976,17 +4978,17 @@
         <f>A20+20</f>
         <v>200</v>
       </c>
-      <c r="B21" s="4">
+      <c r="B21" s="6">
         <v>153371.8199</v>
       </c>
-      <c r="C21" s="4">
+      <c r="C21" s="11">
         <f t="shared" si="0"/>
         <v>153.37181989999999</v>
       </c>
       <c r="D21" s="6">
         <v>2802.7859450000001</v>
       </c>
-      <c r="E21" s="4">
+      <c r="E21" s="11">
         <f t="shared" si="1"/>
         <v>2.8027859450000001</v>
       </c>
@@ -4994,11 +4996,11 @@
         <f t="shared" si="4"/>
         <v>1.8274451896231298E-2</v>
       </c>
-      <c r="G21" s="4">
+      <c r="G21" s="11">
         <f t="shared" si="2"/>
         <v>46.628180100000009</v>
       </c>
-      <c r="H21" s="4">
+      <c r="H21" s="11">
         <f t="shared" si="3"/>
         <v>0.85210443424625959</v>
       </c>
@@ -5010,17 +5012,17 @@
       <c r="A22" s="3">
         <v>225</v>
       </c>
-      <c r="B22" s="4">
+      <c r="B22" s="6">
         <v>176206.07860000001</v>
       </c>
-      <c r="C22" s="4">
+      <c r="C22" s="11">
         <f t="shared" si="0"/>
         <v>176.20607860000001</v>
       </c>
       <c r="D22" s="6">
         <v>5182.4459409999999</v>
       </c>
-      <c r="E22" s="4">
+      <c r="E22" s="11">
         <f t="shared" si="1"/>
         <v>5.1824459410000001</v>
       </c>
@@ -5028,11 +5030,11 @@
         <f t="shared" ref="F22:F23" si="5">E22/C22</f>
         <v>2.9411277875177683E-2</v>
       </c>
-      <c r="G22" s="4">
+      <c r="G22" s="11">
         <f>A22-C22</f>
         <v>48.793921399999988</v>
       </c>
-      <c r="H22" s="4">
+      <c r="H22" s="11">
         <f t="shared" ref="H22:H23" si="6">F22*G22</f>
         <v>1.4350915809149785</v>
       </c>
@@ -5044,17 +5046,17 @@
       <c r="A23" s="3">
         <v>250</v>
       </c>
-      <c r="B23" s="4">
+      <c r="B23" s="6">
         <v>199321.26560000001</v>
       </c>
-      <c r="C23" s="4">
+      <c r="C23" s="11">
         <f t="shared" si="0"/>
         <v>199.3212656</v>
       </c>
       <c r="D23" s="6">
         <v>3253.5442229999999</v>
       </c>
-      <c r="E23" s="4">
+      <c r="E23" s="11">
         <f t="shared" si="1"/>
         <v>3.253544223</v>
       </c>
@@ -5062,11 +5064,11 @@
         <f t="shared" si="5"/>
         <v>1.6323116418140986E-2</v>
       </c>
-      <c r="G23" s="4">
+      <c r="G23" s="11">
         <f t="shared" ref="G23" si="7">A23-C23</f>
         <v>50.678734399999996</v>
       </c>
-      <c r="H23" s="4">
+      <c r="H23" s="11">
         <f t="shared" si="6"/>
         <v>0.82723488153524627</v>
       </c>

</xml_diff>